<commit_message>
GITBOOK-147: change request with no subject merged in GitBook
</commit_message>
<xml_diff>
--- a/.gitbook/assets/batch-operaties-publicaties-voorbeeld.xlsx
+++ b/.gitbook/assets/batch-operaties-publicaties-voorbeeld.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mietclaes/Documents/UGent/P - Biblio/Features and bugs/batch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mietclaes/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C3512A-D1C8-9E42-A23B-C05000B4A4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E01C5E7-5763-8A42-B55E-BF68BC6D7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FCD81E33-4A21-E240-A451-ED31D55A991D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17500" xr2:uid="{FCD81E33-4A21-E240-A451-ED31D55A991D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="29">
   <si>
     <t>,</t>
   </si>
@@ -84,6 +84,45 @@
   </si>
   <si>
     <t>Maximum 500 regels</t>
+  </si>
+  <si>
+    <t>journal_title.set</t>
+  </si>
+  <si>
+    <t>journal_abbreviation.set</t>
+  </si>
+  <si>
+    <t>isbn.add</t>
+  </si>
+  <si>
+    <t>eisbn.add</t>
+  </si>
+  <si>
+    <t>issn.add</t>
+  </si>
+  <si>
+    <t>eissn.add</t>
+  </si>
+  <si>
+    <t>isbn.remove</t>
+  </si>
+  <si>
+    <t>eisbn.remove</t>
+  </si>
+  <si>
+    <t>issn.remove</t>
+  </si>
+  <si>
+    <t>eissn.remove</t>
+  </si>
+  <si>
+    <t>0268-1161</t>
+  </si>
+  <si>
+    <t>"my journal abbreviation"</t>
+  </si>
+  <si>
+    <t>"my journal"</t>
   </si>
 </sst>
 </file>
@@ -141,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -153,9 +192,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -171,7 +213,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD3C6FA-241F-9845-8619-5E4C25B56ED9}">
-  <dimension ref="A1:F502"/>
+  <dimension ref="A1:F505"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -605,86 +647,176 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -692,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -700,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -708,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -716,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -724,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -732,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -740,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -748,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -756,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>0</v>
       </c>
@@ -764,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -772,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -780,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -788,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -796,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -4556,14 +4688,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:4" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A502" s="4" t="s">
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B502" t="s">
+        <v>0</v>
+      </c>
+      <c r="D502" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B503" t="s">
+        <v>0</v>
+      </c>
+      <c r="D503" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B504" t="s">
+        <v>0</v>
+      </c>
+      <c r="D504" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A505" s="4" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A502:XFD502"/>
+    <mergeCell ref="A505:XFD505"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>